<commit_message>
test cases 3 and 4
</commit_message>
<xml_diff>
--- a/com.apartments/src/test/resources/test_data_apartments.xlsx
+++ b/com.apartments/src/test/resources/test_data_apartments.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.apartments/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFAD0CF-BB13-A74F-939D-F1B1BA07E1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D85078-0119-BC42-B418-17538C1D5AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" activeTab="1" xr2:uid="{21AFA41A-4244-444C-A152-0A848FA08C37}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" activeTab="3" xr2:uid="{21AFA41A-4244-444C-A152-0A848FA08C37}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
     <sheet name="DetailedSearch" sheetId="2" r:id="rId2"/>
+    <sheet name="NumOfFavorites" sheetId="3" r:id="rId3"/>
+    <sheet name="OneFavorite" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Manhattan, NY</t>
   </si>
@@ -48,14 +50,20 @@
     <t>Queens, NY</t>
   </si>
   <si>
-    <t>Apartment for Rent</t>
+    <t>Halletts Point</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -66,6 +74,11 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
@@ -90,9 +103,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,21 +448,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7ADF543-C6CE-0A4C-9DCF-2C13A79E6F0D}">
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715103B8-2FF7-D54C-98F8-CCB41440DEFF}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DC07FF-384D-1C43-8A2B-3B8B579B007B}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>